<commit_message>
Preparing for another run through session.  Cleaned up results by plancing in an ignored folder.
</commit_message>
<xml_diff>
--- a/kappa_check.xlsx
+++ b/kappa_check.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/walterstock3/Source/BU_CS699_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14F9178D-322F-B249-B01D-CE4927A8F25E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5E9A60-071B-EC4E-BA8A-1D6A7C5FE5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38340" yWindow="-43000" windowWidth="27240" windowHeight="16440" xr2:uid="{5548BFD4-3BCE-2446-959A-588B4ADE9DB8}"/>
+    <workbookView xWindow="4060" yWindow="3160" windowWidth="27240" windowHeight="16440" xr2:uid="{5548BFD4-3BCE-2446-959A-588B4ADE9DB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="4">
   <si>
     <t>po0</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>k0</t>
+  </si>
+  <si>
+    <t>precision</t>
   </si>
 </sst>
 </file>
@@ -431,15 +434,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D2D0CB8-A0BF-4644-92E3-017D1774C61A}">
-  <dimension ref="C8:U18"/>
+  <dimension ref="C8:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.6640625" bestFit="1" customWidth="1"/>
@@ -757,6 +760,19 @@
         <v>0.8</v>
       </c>
     </row>
+    <row r="21" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <f>C10/(C10+D10)</f>
+        <v>0.98346055979643765</v>
+      </c>
+      <c r="I21">
+        <f>H10/(H10+I10)</f>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>